<commit_message>
Added context to top of scripts for publication. Produced anova tables for leaf disc necrosis results
</commit_message>
<xml_diff>
--- a/Data/leaf_surface_data.xlsx
+++ b/Data/leaf_surface_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madisonplunkert/Documents/GitHub/Leaf-surface-traits-2024/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB773A-3659-4D40-B265-712C5DD0740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D58B60F-9765-6F4C-A20E-45E41DA732EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="740" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7100" yWindow="740" windowWidth="29400" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$149</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="353">
   <si>
     <t>pop.code</t>
   </si>
@@ -1050,6 +1051,51 @@
   </si>
   <si>
     <t>0795</t>
+  </si>
+  <si>
+    <t>Column name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>leaf node (numbered with cotyledonary node as 0 and first true leaf node as node 1) from which a leaf was sampled for stomatal peels</t>
+  </si>
+  <si>
+    <t>leaf node (numbered with cotyledonary node as 0 and first true leaf node as node 1) from which a leaf was sampled for contact angle measurement</t>
+  </si>
+  <si>
+    <t>leaf node (numbered with cotyledonary node as 0 and first true leaf node as node 1) from which a leaf was sampled for leaf water droplet adhesion assay, LMA, and succulence</t>
+  </si>
+  <si>
+    <t>mass of leaf immediately after detaching from a well-watered plant</t>
+  </si>
+  <si>
+    <t>last 4 characters of file name for image of water drop on adaxial leaf surface</t>
+  </si>
+  <si>
+    <t>last 4 characters of file name for image of water drop on abaxial leaf surface</t>
+  </si>
+  <si>
+    <t>notes regarding previous columns</t>
+  </si>
+  <si>
+    <t>notes regarding leaf dry mass</t>
+  </si>
+  <si>
+    <t>mass of leaf after submerging in dH2O for 10 seconds and allowing water to run off for 10 seconds, in grams</t>
+  </si>
+  <si>
+    <t>date that leaves were collected for stomatal traits and wettability traits. m/d/y format</t>
+  </si>
+  <si>
+    <t>dry leaf mass in grams</t>
+  </si>
+  <si>
+    <t>file name for image of water drop on adaxial leaf surface</t>
+  </si>
+  <si>
+    <t>file name for image of water drop on abaxial leaf surface</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1106,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d&quot;/&quot;yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1070,6 +1116,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1095,13 +1148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,11 +1376,11 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O118" sqref="O118"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12760,4 +12814,155 @@
   <autoFilter ref="A1:O149" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1C7975-6486-2B45-A962-4BFA875E74FE}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>